<commit_message>
Formatted Round 10 Spreadsheet
</commit_message>
<xml_diff>
--- a/2018SuperRugby/Weekly Forecasts/Round_10.xlsx
+++ b/2018SuperRugby/Weekly Forecasts/Round_10.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RugbyPredictifier\2018SuperRugby\Weekly Forecasts\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Friday" sheetId="1" r:id="rId1"/>
     <sheet name="Saturday" sheetId="2" r:id="rId2"/>
     <sheet name="Sunday" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="49">
   <si>
     <t>City</t>
   </si>
@@ -168,14 +174,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="#0.00"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="#0%"/>
     <numFmt numFmtId="167" formatCode="#0"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -402,12 +408,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -444,12 +444,26 @@
     <xf numFmtId="0" fontId="11" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -496,7 +510,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -528,9 +542,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -562,6 +594,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -737,7 +787,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BI28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -745,9 +795,15 @@
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="25.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="1.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.453125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:61">
+    <row r="1" spans="1:61" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>27</v>
       </c>
@@ -770,599 +826,455 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:61">
+    <row r="2" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="E2" s="6" t="s">
+      <c r="C2" s="18"/>
+      <c r="E2" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="6"/>
-    </row>
-    <row r="3" spans="1:61">
+      <c r="F2" s="18"/>
+    </row>
+    <row r="3" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="7">
-        <v>0.5333358719575877</v>
-      </c>
-      <c r="C3" s="7"/>
-      <c r="E3" s="7">
-        <v>0.5779847760972098</v>
-      </c>
-      <c r="F3" s="7"/>
-    </row>
-    <row r="4" spans="1:61">
+      <c r="B3" s="19">
+        <v>0.53333587195758769</v>
+      </c>
+      <c r="C3" s="19"/>
+      <c r="E3" s="19">
+        <v>0.57798477609720977</v>
+      </c>
+      <c r="F3" s="19"/>
+    </row>
+    <row r="4" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="7">
-        <v>0.7774155012510465</v>
-      </c>
-      <c r="C4" s="7"/>
-      <c r="E4" s="7">
-        <v>0.9425719508746364</v>
-      </c>
-      <c r="F4" s="7"/>
-    </row>
-    <row r="5" spans="1:61">
+      <c r="B4" s="19">
+        <v>0.77741550125104653</v>
+      </c>
+      <c r="C4" s="19"/>
+      <c r="E4" s="19">
+        <v>0.94257195087463641</v>
+      </c>
+      <c r="F4" s="19"/>
+    </row>
+    <row r="5" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="6">
-        <v>41.4623574233072</v>
-      </c>
-      <c r="C5" s="6"/>
-      <c r="E5" s="6">
-        <v>54.47922379817869</v>
-      </c>
-      <c r="F5" s="6"/>
-    </row>
-    <row r="6" spans="1:61">
+      <c r="B5" s="18">
+        <v>41.462357423307203</v>
+      </c>
+      <c r="C5" s="18"/>
+      <c r="E5" s="18">
+        <v>54.479223798178687</v>
+      </c>
+      <c r="F5" s="18"/>
+    </row>
+    <row r="6" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="8">
-        <v>0.2253162</v>
-      </c>
-      <c r="C6" s="8">
-        <v>0.7557762</v>
-      </c>
-      <c r="E6" s="8">
-        <v>0.6269130000000001</v>
-      </c>
-      <c r="F6" s="8">
-        <v>0.3524336</v>
-      </c>
-    </row>
-    <row r="7" spans="1:61">
+      <c r="B6" s="6">
+        <v>0.22531619999999999</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0.75577620000000001</v>
+      </c>
+      <c r="E6" s="6">
+        <v>0.62691300000000005</v>
+      </c>
+      <c r="F6" s="6">
+        <v>0.35243360000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="9">
-        <v>25.1186806</v>
-      </c>
-      <c r="C7" s="9">
+      <c r="B7" s="7">
+        <v>25.118680600000001</v>
+      </c>
+      <c r="C7" s="7">
         <v>40.5380672</v>
       </c>
-      <c r="E7" s="9">
-        <v>45.346999</v>
-      </c>
-      <c r="F7" s="9">
-        <v>36.8164162</v>
-      </c>
-    </row>
-    <row r="8" spans="1:61">
+      <c r="E7" s="7">
+        <v>45.346998999999997</v>
+      </c>
+      <c r="F7" s="7">
+        <v>36.816416199999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="7">
         <v>6</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="7">
         <v>15</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="7">
         <v>19</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="7">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:61">
+    <row r="9" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="7">
         <v>8</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="7">
         <v>20</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="7">
         <v>23</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="7">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:61">
+    <row r="10" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="7">
         <v>11</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="7">
         <v>23</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="7">
         <v>27</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="7">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:61">
+    <row r="11" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11" s="7">
         <v>14</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="7">
         <v>26</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="7">
         <v>30</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="7">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:61">
+    <row r="12" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12" s="7">
         <v>16</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="7">
         <v>28</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="7">
         <v>33</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F12" s="7">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:61">
+    <row r="13" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B13" s="7">
         <v>17</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="7">
         <v>31</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E13" s="7">
         <v>35</v>
       </c>
-      <c r="F13" s="9">
+      <c r="F13" s="7">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:61">
+    <row r="14" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="9">
+      <c r="B14" s="7">
         <v>19</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="7">
         <v>33</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="7">
         <v>38</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F14" s="7">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:61">
+    <row r="15" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B15" s="7">
         <v>20</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="7">
         <v>35</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15" s="7">
         <v>40</v>
       </c>
-      <c r="F15" s="9">
+      <c r="F15" s="7">
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:61">
+    <row r="16" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="9">
+      <c r="B16" s="7">
         <v>22</v>
       </c>
-      <c r="C16" s="9">
+      <c r="C16" s="7">
         <v>38</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E16" s="7">
         <v>41</v>
       </c>
-      <c r="F16" s="9">
+      <c r="F16" s="7">
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="9">
+      <c r="B17" s="7">
         <v>24</v>
       </c>
-      <c r="C17" s="9">
+      <c r="C17" s="7">
         <v>39</v>
       </c>
-      <c r="E17" s="9">
+      <c r="E17" s="7">
         <v>44</v>
       </c>
-      <c r="F17" s="9">
+      <c r="F17" s="7">
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="9">
+      <c r="B18" s="7">
         <v>25</v>
       </c>
-      <c r="C18" s="9">
+      <c r="C18" s="7">
         <v>41</v>
       </c>
-      <c r="E18" s="9">
+      <c r="E18" s="7">
         <v>46</v>
       </c>
-      <c r="F18" s="9">
+      <c r="F18" s="7">
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="9">
+      <c r="B19" s="7">
         <v>27</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C19" s="7">
         <v>44</v>
       </c>
-      <c r="E19" s="9">
+      <c r="E19" s="7">
         <v>49</v>
       </c>
-      <c r="F19" s="9">
+      <c r="F19" s="7">
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="9">
+      <c r="B20" s="7">
         <v>30</v>
       </c>
-      <c r="C20" s="9">
+      <c r="C20" s="7">
         <v>46</v>
       </c>
-      <c r="E20" s="9">
+      <c r="E20" s="7">
         <v>51</v>
       </c>
-      <c r="F20" s="9">
+      <c r="F20" s="7">
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="9">
+      <c r="B21" s="7">
         <v>32</v>
       </c>
-      <c r="C21" s="9">
+      <c r="C21" s="7">
         <v>49</v>
       </c>
-      <c r="E21" s="9">
+      <c r="E21" s="7">
         <v>54</v>
       </c>
-      <c r="F21" s="9">
+      <c r="F21" s="7">
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="9">
+      <c r="B22" s="7">
         <v>33</v>
       </c>
-      <c r="C22" s="9">
+      <c r="C22" s="7">
         <v>51</v>
       </c>
-      <c r="E22" s="9">
+      <c r="E22" s="7">
         <v>57</v>
       </c>
-      <c r="F22" s="9">
+      <c r="F22" s="7">
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="9">
+      <c r="B23" s="7">
         <v>35</v>
       </c>
-      <c r="C23" s="9">
+      <c r="C23" s="7">
         <v>54</v>
       </c>
-      <c r="E23" s="9">
+      <c r="E23" s="7">
         <v>60</v>
       </c>
-      <c r="F23" s="9">
+      <c r="F23" s="7">
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="9">
+      <c r="B24" s="7">
         <v>39</v>
       </c>
-      <c r="C24" s="9">
+      <c r="C24" s="7">
         <v>58</v>
       </c>
-      <c r="E24" s="9">
+      <c r="E24" s="7">
         <v>64</v>
       </c>
-      <c r="F24" s="9">
+      <c r="F24" s="7">
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="9">
+      <c r="B25" s="7">
         <v>43</v>
       </c>
-      <c r="C25" s="9">
+      <c r="C25" s="7">
         <v>63</v>
       </c>
-      <c r="E25" s="9">
+      <c r="E25" s="7">
         <v>69</v>
       </c>
-      <c r="F25" s="9">
+      <c r="F25" s="7">
         <v>59</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="9">
+      <c r="B26" s="7">
         <v>49</v>
       </c>
-      <c r="C26" s="9">
+      <c r="C26" s="7">
         <v>70</v>
       </c>
-      <c r="E26" s="9">
+      <c r="E26" s="7">
         <v>77</v>
       </c>
-      <c r="F26" s="9">
+      <c r="F26" s="7">
         <v>66</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="8">
-        <v>0.0504428</v>
-      </c>
-      <c r="C27" s="8">
-        <v>0.3817722</v>
-      </c>
-      <c r="E27" s="8">
-        <v>0.2137682</v>
-      </c>
-      <c r="F27" s="8">
-        <v>0.186988</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+      <c r="B27" s="6">
+        <v>5.0442800000000003E-2</v>
+      </c>
+      <c r="C27" s="6">
+        <v>0.38177220000000001</v>
+      </c>
+      <c r="E27" s="6">
+        <v>0.21376819999999999</v>
+      </c>
+      <c r="F27" s="6">
+        <v>0.18698799999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="8">
-        <v>0.1112878</v>
-      </c>
-      <c r="C28" s="8">
-        <v>0.08339580000000001</v>
-      </c>
-      <c r="E28" s="8">
-        <v>0.0966142</v>
-      </c>
-      <c r="F28" s="8">
-        <v>0.1085756</v>
+      <c r="B28" s="6">
+        <v>0.11128780000000001</v>
+      </c>
+      <c r="C28" s="6">
+        <v>8.3395800000000006E-2</v>
+      </c>
+      <c r="E28" s="6">
+        <v>9.6614199999999997E-2</v>
+      </c>
+      <c r="F28" s="6">
+        <v>0.10857559999999999</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="152">
+  <mergeCells count="8">
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E4:F4"/>
@@ -1373,7 +1285,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BI28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1381,40 +1293,49 @@
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="25.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="1.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="1.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="1.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.90625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:61">
-      <c r="B1" s="10" t="s">
+    <row r="1" spans="1:61" x14ac:dyDescent="0.35">
+      <c r="B1" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="9" t="s">
         <v>35</v>
       </c>
       <c r="D1" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="11" t="s">
         <v>38</v>
       </c>
       <c r="G1" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="13" t="s">
         <v>41</v>
       </c>
       <c r="J1" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="16" t="s">
+      <c r="K1" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="L1" s="17" t="s">
+      <c r="L1" s="15" t="s">
         <v>44</v>
       </c>
       <c r="M1" t="s">
@@ -1424,831 +1345,763 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:61">
+    <row r="2" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="E2" s="6" t="s">
+      <c r="C2" s="18"/>
+      <c r="E2" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="F2" s="6"/>
-      <c r="H2" s="6" t="s">
+      <c r="F2" s="18"/>
+      <c r="H2" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="I2" s="6"/>
-      <c r="K2" s="6" t="s">
+      <c r="I2" s="18"/>
+      <c r="K2" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="L2" s="6"/>
-    </row>
-    <row r="3" spans="1:61">
+      <c r="L2" s="18"/>
+    </row>
+    <row r="3" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="7">
-        <v>0.4698381408168071</v>
-      </c>
-      <c r="C3" s="7"/>
-      <c r="E3" s="7">
+      <c r="B3" s="19">
+        <v>0.46983814081680708</v>
+      </c>
+      <c r="C3" s="19"/>
+      <c r="E3" s="19">
         <v>0.4676989577108569</v>
       </c>
-      <c r="F3" s="7"/>
-      <c r="H3" s="7">
-        <v>0.5911992428867379</v>
-      </c>
-      <c r="I3" s="7"/>
-      <c r="K3" s="7">
-        <v>0.3348173655171117</v>
-      </c>
-      <c r="L3" s="7"/>
-    </row>
-    <row r="4" spans="1:61">
+      <c r="F3" s="19"/>
+      <c r="H3" s="19">
+        <v>0.59119924288673786</v>
+      </c>
+      <c r="I3" s="19"/>
+      <c r="K3" s="19">
+        <v>0.33481736551711172</v>
+      </c>
+      <c r="L3" s="19"/>
+    </row>
+    <row r="4" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="7">
-        <v>0.3160981304783388</v>
-      </c>
-      <c r="C4" s="7"/>
-      <c r="E4" s="7">
+      <c r="B4" s="19">
+        <v>0.31609813047833879</v>
+      </c>
+      <c r="C4" s="19"/>
+      <c r="E4" s="19">
         <v>0.730084099126732</v>
       </c>
-      <c r="F4" s="7"/>
-      <c r="H4" s="7">
-        <v>0.9976269142211622</v>
-      </c>
-      <c r="I4" s="7"/>
-      <c r="K4" s="7">
+      <c r="F4" s="19"/>
+      <c r="H4" s="19">
+        <v>0.99762691422116223</v>
+      </c>
+      <c r="I4" s="19"/>
+      <c r="K4" s="19">
         <v>0.9997782487343172</v>
       </c>
-      <c r="L4" s="7"/>
-    </row>
-    <row r="5" spans="1:61">
+      <c r="L4" s="19"/>
+    </row>
+    <row r="5" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="6">
-        <v>14.85149579396112</v>
-      </c>
-      <c r="C5" s="6"/>
-      <c r="E5" s="6">
-        <v>34.14595722028425</v>
-      </c>
-      <c r="F5" s="6"/>
-      <c r="H5" s="6">
-        <v>58.97962763709837</v>
-      </c>
-      <c r="I5" s="6"/>
-      <c r="K5" s="6">
-        <v>33.47431193425356</v>
-      </c>
-      <c r="L5" s="6"/>
-    </row>
-    <row r="6" spans="1:61">
+      <c r="B5" s="18">
+        <v>14.851495793961121</v>
+      </c>
+      <c r="C5" s="18"/>
+      <c r="E5" s="18">
+        <v>34.145957220284252</v>
+      </c>
+      <c r="F5" s="18"/>
+      <c r="H5" s="18">
+        <v>58.979627637098368</v>
+      </c>
+      <c r="I5" s="18"/>
+      <c r="K5" s="18">
+        <v>33.474311934253564</v>
+      </c>
+      <c r="L5" s="18"/>
+    </row>
+    <row r="6" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="8">
-        <v>0.9349582</v>
-      </c>
-      <c r="C6" s="8">
-        <v>0.0566904</v>
-      </c>
-      <c r="E6" s="8">
-        <v>0.199889</v>
-      </c>
-      <c r="F6" s="8">
-        <v>0.7794022</v>
-      </c>
-      <c r="H6" s="8">
-        <v>0.4610202</v>
-      </c>
-      <c r="I6" s="8">
-        <v>0.517107</v>
-      </c>
-      <c r="K6" s="8">
+      <c r="B6" s="6">
+        <v>0.93495819999999996</v>
+      </c>
+      <c r="C6" s="6">
+        <v>5.6690400000000002E-2</v>
+      </c>
+      <c r="E6" s="6">
+        <v>0.19988900000000001</v>
+      </c>
+      <c r="F6" s="6">
+        <v>0.77940220000000004</v>
+      </c>
+      <c r="H6" s="6">
+        <v>0.46102019999999999</v>
+      </c>
+      <c r="I6" s="6">
+        <v>0.51710699999999998</v>
+      </c>
+      <c r="K6" s="6">
         <v>0.4977472</v>
       </c>
-      <c r="L6" s="8">
-        <v>0.4805942</v>
-      </c>
-    </row>
-    <row r="7" spans="1:61">
+      <c r="L6" s="6">
+        <v>0.48059420000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="9">
-        <v>52.9089402</v>
-      </c>
-      <c r="C7" s="9">
-        <v>18.2685462</v>
-      </c>
-      <c r="E7" s="9">
-        <v>18.8818526</v>
-      </c>
-      <c r="F7" s="9">
-        <v>34.2412352</v>
-      </c>
-      <c r="H7" s="9">
+      <c r="B7" s="7">
+        <v>52.908940200000004</v>
+      </c>
+      <c r="C7" s="7">
+        <v>18.268546199999999</v>
+      </c>
+      <c r="E7" s="7">
+        <v>18.881852599999998</v>
+      </c>
+      <c r="F7" s="7">
+        <v>34.241235199999998</v>
+      </c>
+      <c r="H7" s="7">
         <v>32.858694</v>
       </c>
-      <c r="I7" s="9">
+      <c r="I7" s="7">
         <v>34.3965204</v>
       </c>
-      <c r="K7" s="9">
-        <v>33.5379674</v>
-      </c>
-      <c r="L7" s="9">
-        <v>32.9374052</v>
-      </c>
-    </row>
-    <row r="8" spans="1:61">
+      <c r="K7" s="7">
+        <v>33.537967399999999</v>
+      </c>
+      <c r="L7" s="7">
+        <v>32.937405200000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="7">
         <v>22</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="7">
         <v>0</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="7">
         <v>3</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="7">
         <v>11</v>
       </c>
-      <c r="H8" s="9">
+      <c r="H8" s="7">
         <v>9</v>
       </c>
-      <c r="I8" s="9">
+      <c r="I8" s="7">
         <v>11</v>
       </c>
-      <c r="K8" s="9">
+      <c r="K8" s="7">
         <v>8</v>
       </c>
-      <c r="L8" s="9">
+      <c r="L8" s="7">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:61">
+    <row r="9" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="7">
         <v>28</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="7">
         <v>3</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="7">
         <v>6</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="7">
         <v>15</v>
       </c>
-      <c r="H9" s="9">
+      <c r="H9" s="7">
         <v>14</v>
       </c>
-      <c r="I9" s="9">
+      <c r="I9" s="7">
         <v>15</v>
       </c>
-      <c r="K9" s="9">
+      <c r="K9" s="7">
         <v>14</v>
       </c>
-      <c r="L9" s="9">
+      <c r="L9" s="7">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:61">
+    <row r="10" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="7">
         <v>32</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="7">
         <v>8</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="7">
         <v>8</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="7">
         <v>17</v>
       </c>
-      <c r="H10" s="9">
+      <c r="H10" s="7">
         <v>17</v>
       </c>
-      <c r="I10" s="9">
+      <c r="I10" s="7">
         <v>18</v>
       </c>
-      <c r="K10" s="9">
+      <c r="K10" s="7">
         <v>16</v>
       </c>
-      <c r="L10" s="9">
+      <c r="L10" s="7">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:61">
+    <row r="11" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11" s="7">
         <v>36</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="7">
         <v>8</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="7">
         <v>9</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="7">
         <v>21</v>
       </c>
-      <c r="H11" s="9">
+      <c r="H11" s="7">
         <v>20</v>
       </c>
-      <c r="I11" s="9">
+      <c r="I11" s="7">
         <v>22</v>
       </c>
-      <c r="K11" s="9">
+      <c r="K11" s="7">
         <v>19</v>
       </c>
-      <c r="L11" s="9">
+      <c r="L11" s="7">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:61">
+    <row r="12" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12" s="7">
         <v>38</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="7">
         <v>9</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="7">
         <v>11</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F12" s="7">
         <v>23</v>
       </c>
-      <c r="H12" s="9">
+      <c r="H12" s="7">
         <v>22</v>
       </c>
-      <c r="I12" s="9">
+      <c r="I12" s="7">
         <v>23</v>
       </c>
-      <c r="K12" s="9">
+      <c r="K12" s="7">
         <v>22</v>
       </c>
-      <c r="L12" s="9">
+      <c r="L12" s="7">
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:61">
+    <row r="13" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B13" s="7">
         <v>42</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="7">
         <v>11</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E13" s="7">
         <v>12</v>
       </c>
-      <c r="F13" s="9">
+      <c r="F13" s="7">
         <v>25</v>
       </c>
-      <c r="H13" s="9">
+      <c r="H13" s="7">
         <v>24</v>
       </c>
-      <c r="I13" s="9">
+      <c r="I13" s="7">
         <v>25</v>
       </c>
-      <c r="K13" s="9">
+      <c r="K13" s="7">
         <v>24</v>
       </c>
-      <c r="L13" s="9">
+      <c r="L13" s="7">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:61">
+    <row r="14" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="9">
+      <c r="B14" s="7">
         <v>44</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="7">
         <v>14</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="7">
         <v>14</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F14" s="7">
         <v>27</v>
       </c>
-      <c r="H14" s="9">
+      <c r="H14" s="7">
         <v>26</v>
       </c>
-      <c r="I14" s="9">
+      <c r="I14" s="7">
         <v>28</v>
       </c>
-      <c r="K14" s="9">
+      <c r="K14" s="7">
         <v>27</v>
       </c>
-      <c r="L14" s="9">
+      <c r="L14" s="7">
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:61">
+    <row r="15" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B15" s="7">
         <v>46</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="7">
         <v>14</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15" s="7">
         <v>15</v>
       </c>
-      <c r="F15" s="9">
+      <c r="F15" s="7">
         <v>30</v>
       </c>
-      <c r="H15" s="9">
+      <c r="H15" s="7">
         <v>28</v>
       </c>
-      <c r="I15" s="9">
+      <c r="I15" s="7">
         <v>30</v>
       </c>
-      <c r="K15" s="9">
+      <c r="K15" s="7">
         <v>28</v>
       </c>
-      <c r="L15" s="9">
+      <c r="L15" s="7">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:61">
+    <row r="16" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="9">
+      <c r="B16" s="7">
         <v>50</v>
       </c>
-      <c r="C16" s="9">
+      <c r="C16" s="7">
         <v>16</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E16" s="7">
         <v>17</v>
       </c>
-      <c r="F16" s="9">
+      <c r="F16" s="7">
         <v>31</v>
       </c>
-      <c r="H16" s="9">
+      <c r="H16" s="7">
         <v>30</v>
       </c>
-      <c r="I16" s="9">
+      <c r="I16" s="7">
         <v>31</v>
       </c>
-      <c r="K16" s="9">
+      <c r="K16" s="7">
         <v>30</v>
       </c>
-      <c r="L16" s="9">
+      <c r="L16" s="7">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="9">
+      <c r="B17" s="7">
         <v>52</v>
       </c>
-      <c r="C17" s="9">
+      <c r="C17" s="7">
         <v>16</v>
       </c>
-      <c r="E17" s="9">
+      <c r="E17" s="7">
         <v>17</v>
       </c>
-      <c r="F17" s="9">
+      <c r="F17" s="7">
         <v>33</v>
       </c>
-      <c r="H17" s="9">
+      <c r="H17" s="7">
         <v>31</v>
       </c>
-      <c r="I17" s="9">
+      <c r="I17" s="7">
         <v>33</v>
       </c>
-      <c r="K17" s="9">
+      <c r="K17" s="7">
         <v>32</v>
       </c>
-      <c r="L17" s="9">
+      <c r="L17" s="7">
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="9">
+      <c r="B18" s="7">
         <v>54</v>
       </c>
-      <c r="C18" s="9">
+      <c r="C18" s="7">
         <v>19</v>
       </c>
-      <c r="E18" s="9">
+      <c r="E18" s="7">
         <v>19</v>
       </c>
-      <c r="F18" s="9">
+      <c r="F18" s="7">
         <v>35</v>
       </c>
-      <c r="H18" s="9">
+      <c r="H18" s="7">
         <v>33</v>
       </c>
-      <c r="I18" s="9">
+      <c r="I18" s="7">
         <v>35</v>
       </c>
-      <c r="K18" s="9">
+      <c r="K18" s="7">
         <v>34</v>
       </c>
-      <c r="L18" s="9">
+      <c r="L18" s="7">
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="9">
+      <c r="B19" s="7">
         <v>56</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C19" s="7">
         <v>19</v>
       </c>
-      <c r="E19" s="9">
+      <c r="E19" s="7">
         <v>20</v>
       </c>
-      <c r="F19" s="9">
+      <c r="F19" s="7">
         <v>38</v>
       </c>
-      <c r="H19" s="9">
+      <c r="H19" s="7">
         <v>36</v>
       </c>
-      <c r="I19" s="9">
+      <c r="I19" s="7">
         <v>37</v>
       </c>
-      <c r="K19" s="9">
+      <c r="K19" s="7">
         <v>36</v>
       </c>
-      <c r="L19" s="9">
+      <c r="L19" s="7">
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="9">
+      <c r="B20" s="7">
         <v>60</v>
       </c>
-      <c r="C20" s="9">
+      <c r="C20" s="7">
         <v>22</v>
       </c>
-      <c r="E20" s="9">
+      <c r="E20" s="7">
         <v>22</v>
       </c>
-      <c r="F20" s="9">
+      <c r="F20" s="7">
         <v>39</v>
       </c>
-      <c r="H20" s="9">
+      <c r="H20" s="7">
         <v>38</v>
       </c>
-      <c r="I20" s="9">
+      <c r="I20" s="7">
         <v>39</v>
       </c>
-      <c r="K20" s="9">
+      <c r="K20" s="7">
         <v>38</v>
       </c>
-      <c r="L20" s="9">
+      <c r="L20" s="7">
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="9">
+      <c r="B21" s="7">
         <v>62</v>
       </c>
-      <c r="C21" s="9">
+      <c r="C21" s="7">
         <v>24</v>
       </c>
-      <c r="E21" s="9">
+      <c r="E21" s="7">
         <v>23</v>
       </c>
-      <c r="F21" s="9">
+      <c r="F21" s="7">
         <v>41</v>
       </c>
-      <c r="H21" s="9">
+      <c r="H21" s="7">
         <v>40</v>
       </c>
-      <c r="I21" s="9">
+      <c r="I21" s="7">
         <v>42</v>
       </c>
-      <c r="K21" s="9">
+      <c r="K21" s="7">
         <v>41</v>
       </c>
-      <c r="L21" s="9">
+      <c r="L21" s="7">
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="9">
+      <c r="B22" s="7">
         <v>66</v>
       </c>
-      <c r="C22" s="9">
+      <c r="C22" s="7">
         <v>25</v>
       </c>
-      <c r="E22" s="9">
+      <c r="E22" s="7">
         <v>25</v>
       </c>
-      <c r="F22" s="9">
+      <c r="F22" s="7">
         <v>44</v>
       </c>
-      <c r="H22" s="9">
+      <c r="H22" s="7">
         <v>42</v>
       </c>
-      <c r="I22" s="9">
+      <c r="I22" s="7">
         <v>44</v>
       </c>
-      <c r="K22" s="9">
+      <c r="K22" s="7">
         <v>43</v>
       </c>
-      <c r="L22" s="9">
+      <c r="L22" s="7">
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="9">
+      <c r="B23" s="7">
         <v>70</v>
       </c>
-      <c r="C23" s="9">
+      <c r="C23" s="7">
         <v>27</v>
       </c>
-      <c r="E23" s="9">
+      <c r="E23" s="7">
         <v>28</v>
       </c>
-      <c r="F23" s="9">
+      <c r="F23" s="7">
         <v>47</v>
       </c>
-      <c r="H23" s="9">
+      <c r="H23" s="7">
         <v>45</v>
       </c>
-      <c r="I23" s="9">
+      <c r="I23" s="7">
         <v>47</v>
       </c>
-      <c r="K23" s="9">
+      <c r="K23" s="7">
         <v>46</v>
       </c>
-      <c r="L23" s="9">
+      <c r="L23" s="7">
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="9">
+      <c r="B24" s="7">
         <v>74</v>
       </c>
-      <c r="C24" s="9">
+      <c r="C24" s="7">
         <v>30</v>
       </c>
-      <c r="E24" s="9">
+      <c r="E24" s="7">
         <v>30</v>
       </c>
-      <c r="F24" s="9">
+      <c r="F24" s="7">
         <v>51</v>
       </c>
-      <c r="H24" s="9">
+      <c r="H24" s="7">
         <v>49</v>
       </c>
-      <c r="I24" s="9">
+      <c r="I24" s="7">
         <v>51</v>
       </c>
-      <c r="K24" s="9">
+      <c r="K24" s="7">
         <v>50</v>
       </c>
-      <c r="L24" s="9">
+      <c r="L24" s="7">
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="9">
+      <c r="B25" s="7">
         <v>80</v>
       </c>
-      <c r="C25" s="9">
+      <c r="C25" s="7">
         <v>33</v>
       </c>
-      <c r="E25" s="9">
+      <c r="E25" s="7">
         <v>33</v>
       </c>
-      <c r="F25" s="9">
+      <c r="F25" s="7">
         <v>55</v>
       </c>
-      <c r="H25" s="9">
+      <c r="H25" s="7">
         <v>53</v>
       </c>
-      <c r="I25" s="9">
+      <c r="I25" s="7">
         <v>55</v>
       </c>
-      <c r="K25" s="9">
+      <c r="K25" s="7">
         <v>54</v>
       </c>
-      <c r="L25" s="9">
+      <c r="L25" s="7">
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="9">
+      <c r="B26" s="7">
         <v>88</v>
       </c>
-      <c r="C26" s="9">
+      <c r="C26" s="7">
         <v>39</v>
       </c>
-      <c r="E26" s="9">
+      <c r="E26" s="7">
         <v>38</v>
       </c>
-      <c r="F26" s="9">
+      <c r="F26" s="7">
         <v>62</v>
       </c>
-      <c r="H26" s="9">
+      <c r="H26" s="7">
         <v>60</v>
       </c>
-      <c r="I26" s="9">
+      <c r="I26" s="7">
         <v>62</v>
       </c>
-      <c r="K26" s="9">
+      <c r="K26" s="7">
         <v>62</v>
       </c>
-      <c r="L26" s="9">
+      <c r="L26" s="7">
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="8">
-        <v>0.7983336</v>
-      </c>
-      <c r="C27" s="8">
-        <v>0.0042316</v>
-      </c>
-      <c r="E27" s="8">
-        <v>0.0095076</v>
-      </c>
-      <c r="F27" s="8">
-        <v>0.5353924</v>
-      </c>
-      <c r="H27" s="8">
-        <v>0.1667204</v>
-      </c>
-      <c r="I27" s="8">
+      <c r="B27" s="6">
+        <v>0.79833359999999998</v>
+      </c>
+      <c r="C27" s="6">
+        <v>4.2316000000000003E-3</v>
+      </c>
+      <c r="E27" s="6">
+        <v>9.5075999999999997E-3</v>
+      </c>
+      <c r="F27" s="6">
+        <v>0.53539239999999999</v>
+      </c>
+      <c r="H27" s="6">
+        <v>0.16672039999999999</v>
+      </c>
+      <c r="I27" s="6">
         <v>0.221246</v>
       </c>
-      <c r="K27" s="8">
+      <c r="K27" s="6">
         <v>0.228186</v>
       </c>
-      <c r="L27" s="8">
-        <v>0.1375686</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12">
+      <c r="L27" s="6">
+        <v>0.13756860000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="8">
-        <v>0.027235</v>
-      </c>
-      <c r="C28" s="8">
-        <v>0.0484154</v>
-      </c>
-      <c r="E28" s="8">
+      <c r="B28" s="6">
+        <v>2.7234999999999999E-2</v>
+      </c>
+      <c r="C28" s="6">
+        <v>4.8415399999999997E-2</v>
+      </c>
+      <c r="E28" s="6">
         <v>0.1222944</v>
       </c>
-      <c r="F28" s="8">
-        <v>0.088287</v>
-      </c>
-      <c r="H28" s="8">
+      <c r="F28" s="6">
+        <v>8.8287000000000004E-2</v>
+      </c>
+      <c r="H28" s="6">
         <v>0.125086</v>
       </c>
-      <c r="I28" s="8">
+      <c r="I28" s="6">
         <v>0.121492</v>
       </c>
-      <c r="K28" s="8">
+      <c r="K28" s="6">
         <v>0.1242844</v>
       </c>
-      <c r="L28" s="8">
+      <c r="L28" s="6">
         <v>0.1238238</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="304">
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
+  <mergeCells count="16">
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K5:L5"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
@@ -2257,237 +2110,17 @@
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="K5:L5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BI28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2495,13 +2128,18 @@
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="25.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.36328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:61">
-      <c r="B1" s="18" t="s">
+    <row r="1" spans="1:61" x14ac:dyDescent="0.35">
+      <c r="B1" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="17" t="s">
         <v>47</v>
       </c>
       <c r="D1" t="s">
@@ -2511,369 +2149,297 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:61">
+    <row r="2" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="6"/>
-    </row>
-    <row r="3" spans="1:61">
+      <c r="C2" s="18"/>
+    </row>
+    <row r="3" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="7">
-        <v>0.292823048735413</v>
-      </c>
-      <c r="C3" s="7"/>
-    </row>
-    <row r="4" spans="1:61">
+      <c r="B3" s="19">
+        <v>0.29282304873541298</v>
+      </c>
+      <c r="C3" s="19"/>
+    </row>
+    <row r="4" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="7">
-        <v>0.9977391419576627</v>
-      </c>
-      <c r="C4" s="7"/>
-    </row>
-    <row r="5" spans="1:61">
+      <c r="B4" s="19">
+        <v>0.99773914195766267</v>
+      </c>
+      <c r="C4" s="19"/>
+    </row>
+    <row r="5" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="6">
-        <v>29.21610173906978</v>
-      </c>
-      <c r="C5" s="6"/>
-    </row>
-    <row r="6" spans="1:61">
+      <c r="B5" s="18">
+        <v>29.216101739069781</v>
+      </c>
+      <c r="C5" s="18"/>
+    </row>
+    <row r="6" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="8">
-        <v>0.5134022</v>
-      </c>
-      <c r="C6" s="8">
-        <v>0.4589786</v>
-      </c>
-    </row>
-    <row r="7" spans="1:61">
+      <c r="B6" s="6">
+        <v>0.51340220000000003</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0.45897860000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="7">
         <v>25.9941338</v>
       </c>
-      <c r="C7" s="9">
-        <v>24.7489966</v>
-      </c>
-    </row>
-    <row r="8" spans="1:61">
+      <c r="C7" s="7">
+        <v>24.748996600000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="7">
         <v>6</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="7">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:61">
+    <row r="9" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="7">
         <v>9</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="7">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:61">
+    <row r="10" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="7">
         <v>12</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="7">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:61">
+    <row r="11" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11" s="7">
         <v>14</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="7">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:61">
+    <row r="12" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12" s="7">
         <v>17</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="7">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:61">
+    <row r="13" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B13" s="7">
         <v>18</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="7">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:61">
+    <row r="14" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="9">
+      <c r="B14" s="7">
         <v>20</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="7">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:61">
+    <row r="15" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B15" s="7">
         <v>22</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="7">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:61">
+    <row r="16" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="9">
+      <c r="B16" s="7">
         <v>23</v>
       </c>
-      <c r="C16" s="9">
+      <c r="C16" s="7">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="9">
+      <c r="B17" s="7">
         <v>25</v>
       </c>
-      <c r="C17" s="9">
+      <c r="C17" s="7">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="9">
+      <c r="B18" s="7">
         <v>26</v>
       </c>
-      <c r="C18" s="9">
+      <c r="C18" s="7">
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="9">
+      <c r="B19" s="7">
         <v>28</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C19" s="7">
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="9">
+      <c r="B20" s="7">
         <v>30</v>
       </c>
-      <c r="C20" s="9">
+      <c r="C20" s="7">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="9">
+      <c r="B21" s="7">
         <v>32</v>
       </c>
-      <c r="C21" s="9">
+      <c r="C21" s="7">
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="9">
+      <c r="B22" s="7">
         <v>34</v>
       </c>
-      <c r="C22" s="9">
+      <c r="C22" s="7">
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="9">
+      <c r="B23" s="7">
         <v>37</v>
       </c>
-      <c r="C23" s="9">
+      <c r="C23" s="7">
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="9">
+      <c r="B24" s="7">
         <v>40</v>
       </c>
-      <c r="C24" s="9">
+      <c r="C24" s="7">
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="9">
+      <c r="B25" s="7">
         <v>43</v>
       </c>
-      <c r="C25" s="9">
+      <c r="C25" s="7">
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="9">
+      <c r="B26" s="7">
         <v>49</v>
       </c>
-      <c r="C26" s="9">
+      <c r="C26" s="7">
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="8">
-        <v>0.2359266</v>
-      </c>
-      <c r="C27" s="8">
-        <v>0.0679582</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
+      <c r="B27" s="6">
+        <v>0.23592659999999999</v>
+      </c>
+      <c r="C27" s="6">
+        <v>6.7958199999999996E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="8">
-        <v>0.1455434</v>
-      </c>
-      <c r="C28" s="8">
-        <v>0.1512798</v>
+      <c r="B28" s="6">
+        <v>0.14554339999999999</v>
+      </c>
+      <c r="C28" s="6">
+        <v>0.15127979999999999</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="76">
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
+  <mergeCells count="4">
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>

</xml_diff>